<commit_message>
Edited R and stan code to use data stored in spreadsheets
</commit_message>
<xml_diff>
--- a/output/processed/sofa/Preytypes.xlsx
+++ b/output/processed/sofa/Preytypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Papers/Monterey_mussel_urchin_otter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{D5682D9A-7EB2-49F5-A684-1D0D3BA1E1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{120AFC54-7B32-4C16-A747-835668F553C4}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{D5682D9A-7EB2-49F5-A684-1D0D3BA1E1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5448C34-C2DD-4EF9-9D9B-03101FAADEC5}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="38700" windowHeight="15345" xr2:uid="{51AEABE2-89C9-42AB-864C-1CA819F72A1B}"/>
+    <workbookView xWindow="5955" yWindow="3135" windowWidth="38700" windowHeight="15345" xr2:uid="{51AEABE2-89C9-42AB-864C-1CA819F72A1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>TypeN</t>
   </si>
@@ -47,12 +47,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Min_size_mm</t>
-  </si>
-  <si>
     <t>gamma1</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>Other crabs</t>
   </si>
   <si>
-    <t>other_crab</t>
-  </si>
-  <si>
     <t>snail</t>
   </si>
   <si>
@@ -134,7 +125,10 @@
     <t>chitons, limpets, barnacles,etc.</t>
   </si>
   <si>
-    <t>other_hardsub</t>
+    <t>log_G_mn</t>
+  </si>
+  <si>
+    <t>log_G_sd</t>
   </si>
 </sst>
 </file>
@@ -187,6 +181,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -509,14 +507,17 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -542,10 +543,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -553,28 +554,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>-9.1557912800493906</v>
       </c>
       <c r="E2">
-        <v>25</v>
+        <v>3.1172105405765098</v>
       </c>
       <c r="F2">
-        <v>-9.1557912800493906</v>
+        <v>-0.28768207245178101</v>
       </c>
       <c r="G2">
-        <v>3.1172105405765098</v>
+        <v>3.7781937069642203E-2</v>
       </c>
       <c r="H2">
-        <v>-0.28768207245178101</v>
+        <v>2.0137508156211599</v>
       </c>
       <c r="I2">
-        <v>3.7781937069642203E-2</v>
+        <v>0.12278231544543</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -582,28 +583,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>-6.1239876951112802</v>
       </c>
       <c r="E3">
-        <v>25</v>
+        <v>2.0835640977838201</v>
       </c>
       <c r="F3">
-        <v>-6.1239876951112802</v>
+        <v>-0.28903109543787397</v>
       </c>
       <c r="G3">
-        <v>2.0835640977838201</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H3">
-        <v>-0.28903109543787397</v>
+        <v>1.3390248208506701</v>
       </c>
       <c r="I3">
-        <v>6.25E-2</v>
+        <v>0.113096287026453</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -611,28 +612,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>-8.6152793977053204</v>
       </c>
       <c r="E4">
-        <v>25</v>
+        <v>2.9069444229797599</v>
       </c>
       <c r="F4">
-        <v>-8.6152793977053204</v>
+        <v>-0.460616762512638</v>
       </c>
       <c r="G4">
-        <v>2.9069444229797599</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H4">
-        <v>-0.460616762512638</v>
+        <v>2.5424261328162698</v>
       </c>
       <c r="I4">
-        <v>6.25E-2</v>
+        <v>0.16728201738732901</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -640,28 +641,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>-7.8250485135578201</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>2.68367446900147</v>
       </c>
       <c r="F5">
-        <v>-7.8250485135578201</v>
+        <v>-1.4228674612371201E-2</v>
       </c>
       <c r="G5">
-        <v>2.68367446900147</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H5">
-        <v>-1.4228674612371201E-2</v>
+        <v>4.5187521446107199</v>
       </c>
       <c r="I5">
-        <v>6.25E-2</v>
+        <v>0.179485506757257</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -669,28 +670,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>-9.27390081238131</v>
       </c>
       <c r="E6">
-        <v>25</v>
+        <v>2.96116021712495</v>
       </c>
       <c r="F6">
-        <v>-9.27390081238131</v>
+        <v>-0.21835233805686899</v>
       </c>
       <c r="G6">
-        <v>2.96116021712495</v>
+        <v>5.45198284024545E-2</v>
       </c>
       <c r="H6">
-        <v>-0.21835233805686899</v>
+        <v>3.55296842843984</v>
       </c>
       <c r="I6">
-        <v>5.45198284024545E-2</v>
+        <v>0.19863749715604201</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -698,28 +699,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>-8.7933118956100103</v>
       </c>
       <c r="E7">
-        <v>30</v>
+        <v>3.05773753996605</v>
       </c>
       <c r="F7">
-        <v>-8.7933118956100103</v>
+        <v>-0.29668997638178901</v>
       </c>
       <c r="G7">
-        <v>3.05773753996605</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H7">
-        <v>-0.29668997638178901</v>
+        <v>2.5546121440275198</v>
       </c>
       <c r="I7">
-        <v>6.25E-2</v>
+        <v>0.167053639049039</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -727,28 +728,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>-7.2107642201959399</v>
       </c>
       <c r="E8">
-        <v>20</v>
+        <v>2.5270538062199299</v>
       </c>
       <c r="F8">
-        <v>-7.2107642201959399</v>
+        <v>-0.232007386024601</v>
       </c>
       <c r="G8">
-        <v>2.5270538062199299</v>
+        <v>6.0578240153726502E-2</v>
       </c>
       <c r="H8">
-        <v>-0.232007386024601</v>
+        <v>1.8655089093095001</v>
       </c>
       <c r="I8">
-        <v>6.0578240153726502E-2</v>
+        <v>0.15020469041586601</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -756,28 +757,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>-7.9596874196781204</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>2.7738228422176801</v>
       </c>
       <c r="F9">
-        <v>-7.9596874196781204</v>
+        <v>3.9100135673743902E-2</v>
       </c>
       <c r="G9">
-        <v>2.7738228422176801</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H9">
-        <v>3.9100135673743902E-2</v>
+        <v>0.76349440856147699</v>
       </c>
       <c r="I9">
-        <v>6.25E-2</v>
+        <v>0.14648191676980599</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -785,28 +786,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>-3.0255056410644898</v>
       </c>
       <c r="E10">
-        <v>30</v>
+        <v>1.6308922912286801</v>
       </c>
       <c r="F10">
-        <v>-3.0255056410644898</v>
+        <v>0.26235164220611601</v>
       </c>
       <c r="G10">
-        <v>1.6308922912286801</v>
+        <v>5.1150470442866899E-2</v>
       </c>
       <c r="H10">
-        <v>0.26235164220611601</v>
+        <v>3.6245099212635998</v>
       </c>
       <c r="I10">
-        <v>5.1150470442866899E-2</v>
+        <v>0.15610395082053299</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -814,28 +815,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>-1.27550564106449</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>1.3127794847699099</v>
       </c>
       <c r="F11">
-        <v>-1.27550564106449</v>
+        <v>5.8955356525265998E-2</v>
       </c>
       <c r="G11">
-        <v>1.3127794847699099</v>
+        <v>6.1018000103057399E-2</v>
       </c>
       <c r="H11">
-        <v>5.8955356525265998E-2</v>
+        <v>4.4069120101129204</v>
       </c>
       <c r="I11">
-        <v>6.1018000103057399E-2</v>
+        <v>0.16003677154114301</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -843,28 +844,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>-5.2186653100931002</v>
       </c>
       <c r="E12">
-        <v>10</v>
+        <v>1.7983291177557701</v>
       </c>
       <c r="F12">
-        <v>-5.2186653100931002</v>
+        <v>-0.74606822028809305</v>
       </c>
       <c r="G12">
-        <v>1.7983291177557701</v>
+        <v>3.85562741815463E-2</v>
       </c>
       <c r="H12">
-        <v>-0.74606822028809305</v>
+        <v>1.44661751795251</v>
       </c>
       <c r="I12">
-        <v>3.85562741815463E-2</v>
+        <v>0.100660297301433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>